<commit_message>
chore: Refactor automail.py for improved readability and maintainability
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -1,91 +1,63 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work_space\Email-Automation-Python\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{022A84CF-B1B8-4DBC-BDC6-D6611055AEAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>Full name</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Đào Duy Thông</t>
-  </si>
-  <si>
-    <t>duythong.ptit@gmail.com</t>
-  </si>
-  <si>
-    <t>Tống Ngọc Kiên</t>
-  </si>
-  <si>
-    <t>tongkien123@gmail.com</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
-    <font>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="6">
+    <font>
+      <name val="Arial"/>
+      <color rgb="FF000000"/>
       <sz val="10"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
       <color rgb="FF000000"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <color rgb="FF0563C1"/>
+      <sz val="11"/>
+      <u val="single"/>
+    </font>
+    <font>
       <name val="Arial"/>
+      <color theme="10"/>
+      <sz val="10"/>
+      <u val="single"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0563C1"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color theme="10"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF1F1F1F"/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
+    </font>
+    <font>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF1F1F1F"/>
+      <sz val="8"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -102,33 +74,92 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -329,74 +360,91 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="31.21875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="31.21875" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" ht="15.75" customHeight="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Full name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="n"/>
+    </row>
+    <row r="2" ht="15.75" customHeight="1">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Đào Duy Thông</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>duythong.ptit@gmail.com</t>
+        </is>
+      </c>
+      <c r="C2" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="C1" s="1"/>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="3"/>
-    </row>
-    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="3"/>
-    </row>
-    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="5"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="3"/>
-    </row>
-    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="3"/>
-    </row>
-    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="5"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="3"/>
-    </row>
-    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="5"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="3"/>
-    </row>
-    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="3"/>
+    </row>
+    <row r="3" ht="15.75" customHeight="1">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Tống Ngọc Kiên</t>
+        </is>
+      </c>
+      <c r="B3" s="4" t="inlineStr">
+        <is>
+          <t>duythong020703@gmail.com</t>
+        </is>
+      </c>
+      <c r="C3" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" ht="15.75" customHeight="1">
+      <c r="A4" s="5" t="n"/>
+      <c r="B4" s="6" t="n"/>
+      <c r="C4" s="3" t="n"/>
+    </row>
+    <row r="5" ht="15.75" customHeight="1">
+      <c r="A5" s="5" t="n"/>
+      <c r="B5" s="4" t="n"/>
+      <c r="C5" s="3" t="n"/>
+    </row>
+    <row r="6" ht="15.75" customHeight="1">
+      <c r="A6" s="5" t="n"/>
+      <c r="B6" s="6" t="n"/>
+      <c r="C6" s="3" t="n"/>
+    </row>
+    <row r="7" ht="15.75" customHeight="1">
+      <c r="A7" s="5" t="n"/>
+      <c r="B7" s="6" t="n"/>
+      <c r="C7" s="3" t="n"/>
+    </row>
+    <row r="8" ht="15.75" customHeight="1">
+      <c r="C8" s="3" t="n"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{478A9CF9-A7F6-4E1A-AE36-27F63EB3A02C}"/>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>